<commit_message>
update to replication package
</commit_message>
<xml_diff>
--- a/RP_icse_2018/RQ2_automation_needs/Q2.1-Q2.5_evaluation_survey.xlsx
+++ b/RP_icse_2018/RQ2_automation_needs/Q2.1-Q2.5_evaluation_survey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\OneDrive\BACHELOR_THESIS\automation-needs-mcr\RP_icse_2018\RQ2_automation_needs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\BA\automation-needs-mcr\RP_icse_2018\RQ2_automation_needs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="199" documentId="8_{B9C4F2CF-4F4E-4412-BF52-83BFBF140693}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{C4B3E8DB-F1F9-49A7-ABF4-6A6AA2011A35}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D38E00-5483-4986-9085-EFFED66FE2EE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" activeTab="3" xr2:uid="{015888E5-A0C9-4DA2-83B9-8E164B8C26A4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" activeTab="2" xr2:uid="{015888E5-A0C9-4DA2-83B9-8E164B8C26A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Q2.1-Q2.5 all Findings" sheetId="1" r:id="rId1"/>
@@ -14403,8 +14403,8 @@
   </sheetPr>
   <dimension ref="A1:F431"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B300" sqref="B300:B303"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="9" x14ac:dyDescent="0.25"/>
@@ -22938,11 +22938,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:F431" xr:uid="{04CDE857-764E-4C96-A7F4-40F2CC181309}">
-    <sortState ref="A8:F431">
-      <sortCondition ref="A7"/>
-    </sortState>
-  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:E4"/>
@@ -22954,11 +22949,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5B3391-1F25-4D33-9C01-8AEAD2183D13}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K319"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B324" sqref="B324"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="9" x14ac:dyDescent="0.25"/>
@@ -23025,7 +23019,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
@@ -23060,7 +23054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
@@ -23095,7 +23089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
@@ -23130,7 +23124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>6</v>
       </c>
@@ -23165,7 +23159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
@@ -23200,7 +23194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>6</v>
       </c>
@@ -23235,7 +23229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>6</v>
       </c>
@@ -23270,7 +23264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>6</v>
       </c>
@@ -23305,7 +23299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>6</v>
       </c>
@@ -23340,7 +23334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>6</v>
       </c>
@@ -23375,7 +23369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>6</v>
       </c>
@@ -23410,7 +23404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>6</v>
       </c>
@@ -23445,7 +23439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>6</v>
       </c>
@@ -23480,7 +23474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>6</v>
       </c>
@@ -23515,7 +23509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>6</v>
       </c>
@@ -23550,7 +23544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>6</v>
       </c>
@@ -23585,7 +23579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>6</v>
       </c>
@@ -23620,7 +23614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>6</v>
       </c>
@@ -23655,7 +23649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>6</v>
       </c>
@@ -23690,7 +23684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>6</v>
       </c>
@@ -23725,7 +23719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>6</v>
       </c>
@@ -23760,7 +23754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>6</v>
       </c>
@@ -23795,7 +23789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>6</v>
       </c>
@@ -23830,7 +23824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>6</v>
       </c>
@@ -23865,7 +23859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>6</v>
       </c>
@@ -23900,7 +23894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>6</v>
       </c>
@@ -23935,7 +23929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>6</v>
       </c>
@@ -23970,7 +23964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>6</v>
       </c>
@@ -24005,7 +23999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>6</v>
       </c>
@@ -24040,7 +24034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>6</v>
       </c>
@@ -24075,7 +24069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>6</v>
       </c>
@@ -24110,7 +24104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>6</v>
       </c>
@@ -24145,7 +24139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>6</v>
       </c>
@@ -24180,7 +24174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>6</v>
       </c>
@@ -24215,7 +24209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>6</v>
       </c>
@@ -24250,7 +24244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>6</v>
       </c>
@@ -24285,7 +24279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>6</v>
       </c>
@@ -24320,7 +24314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>6</v>
       </c>
@@ -24355,7 +24349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>6</v>
       </c>
@@ -24390,7 +24384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>6</v>
       </c>
@@ -24425,7 +24419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>6</v>
       </c>
@@ -24460,7 +24454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>6</v>
       </c>
@@ -24495,7 +24489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>6</v>
       </c>
@@ -24530,7 +24524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>6</v>
       </c>
@@ -24565,7 +24559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>6</v>
       </c>
@@ -24600,7 +24594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>6</v>
       </c>
@@ -24635,7 +24629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>6</v>
       </c>
@@ -24670,7 +24664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>6</v>
       </c>
@@ -24705,7 +24699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>6</v>
       </c>
@@ -24740,7 +24734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>6</v>
       </c>
@@ -24775,7 +24769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>6</v>
       </c>
@@ -24810,7 +24804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>6</v>
       </c>
@@ -24845,7 +24839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>6</v>
       </c>
@@ -24880,7 +24874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
         <v>6</v>
       </c>
@@ -24915,7 +24909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
         <v>6</v>
       </c>
@@ -24950,7 +24944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>6</v>
       </c>
@@ -24985,7 +24979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>6</v>
       </c>
@@ -25020,7 +25014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>6</v>
       </c>
@@ -25055,7 +25049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>6</v>
       </c>
@@ -25090,7 +25084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>6</v>
       </c>
@@ -25125,7 +25119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>6</v>
       </c>
@@ -25160,7 +25154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>279</v>
       </c>
@@ -25195,7 +25189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>279</v>
       </c>
@@ -25230,7 +25224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>279</v>
       </c>
@@ -25265,7 +25259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>279</v>
       </c>
@@ -25300,7 +25294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>279</v>
       </c>
@@ -25335,7 +25329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>279</v>
       </c>
@@ -25370,7 +25364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>279</v>
       </c>
@@ -25405,7 +25399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>279</v>
       </c>
@@ -25440,7 +25434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>279</v>
       </c>
@@ -25475,7 +25469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>279</v>
       </c>
@@ -25510,7 +25504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>279</v>
       </c>
@@ -25545,7 +25539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
         <v>279</v>
       </c>
@@ -25580,7 +25574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>279</v>
       </c>
@@ -25615,7 +25609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>279</v>
       </c>
@@ -25650,7 +25644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>279</v>
       </c>
@@ -25685,7 +25679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
         <v>279</v>
       </c>
@@ -25720,7 +25714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
         <v>279</v>
       </c>
@@ -25755,7 +25749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>279</v>
       </c>
@@ -25790,7 +25784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>279</v>
       </c>
@@ -25825,7 +25819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
         <v>279</v>
       </c>
@@ -25860,7 +25854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
         <v>279</v>
       </c>
@@ -25895,7 +25889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
         <v>279</v>
       </c>
@@ -25930,7 +25924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
         <v>279</v>
       </c>
@@ -25965,7 +25959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
         <v>279</v>
       </c>
@@ -26000,7 +25994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
         <v>279</v>
       </c>
@@ -26035,7 +26029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
         <v>279</v>
       </c>
@@ -26070,7 +26064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
         <v>279</v>
       </c>
@@ -26105,7 +26099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
         <v>279</v>
       </c>
@@ -26140,7 +26134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
         <v>279</v>
       </c>
@@ -26175,7 +26169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
         <v>279</v>
       </c>
@@ -26210,7 +26204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
         <v>279</v>
       </c>
@@ -26245,7 +26239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
         <v>279</v>
       </c>
@@ -26280,7 +26274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
         <v>279</v>
       </c>
@@ -26315,7 +26309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
         <v>279</v>
       </c>
@@ -26350,7 +26344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
         <v>279</v>
       </c>
@@ -26385,7 +26379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
         <v>279</v>
       </c>
@@ -26420,7 +26414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
         <v>279</v>
       </c>
@@ -26455,7 +26449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
         <v>279</v>
       </c>
@@ -26490,7 +26484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
         <v>279</v>
       </c>
@@ -26525,7 +26519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
         <v>7</v>
       </c>
@@ -26560,7 +26554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
         <v>7</v>
       </c>
@@ -26595,7 +26589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
         <v>7</v>
       </c>
@@ -26630,7 +26624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
         <v>7</v>
       </c>
@@ -26665,7 +26659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
         <v>7</v>
       </c>
@@ -26700,7 +26694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
         <v>7</v>
       </c>
@@ -26735,7 +26729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
         <v>7</v>
       </c>
@@ -26770,7 +26764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
         <v>7</v>
       </c>
@@ -26805,7 +26799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="11" t="s">
         <v>7</v>
       </c>
@@ -26840,7 +26834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="11" t="s">
         <v>7</v>
       </c>
@@ -26875,7 +26869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="11" t="s">
         <v>7</v>
       </c>
@@ -26910,7 +26904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="11" t="s">
         <v>7</v>
       </c>
@@ -26945,7 +26939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="11" t="s">
         <v>7</v>
       </c>
@@ -26980,7 +26974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
         <v>7</v>
       </c>
@@ -27015,7 +27009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="11" t="s">
         <v>7</v>
       </c>
@@ -27050,7 +27044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="11" t="s">
         <v>7</v>
       </c>
@@ -27085,7 +27079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
         <v>7</v>
       </c>
@@ -27120,7 +27114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
         <v>7</v>
       </c>
@@ -27155,7 +27149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="11" t="s">
         <v>7</v>
       </c>
@@ -27190,7 +27184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A127" s="11" t="s">
         <v>7</v>
       </c>
@@ -27225,7 +27219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A128" s="11" t="s">
         <v>7</v>
       </c>
@@ -27260,7 +27254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
         <v>7</v>
       </c>
@@ -27295,7 +27289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A130" s="11" t="s">
         <v>7</v>
       </c>
@@ -27330,7 +27324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
         <v>7</v>
       </c>
@@ -27365,7 +27359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
         <v>7</v>
       </c>
@@ -27400,7 +27394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="11" t="s">
         <v>7</v>
       </c>
@@ -27435,7 +27429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:11" s="14" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
         <v>7</v>
       </c>
@@ -27470,7 +27464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
         <v>7</v>
       </c>
@@ -27505,7 +27499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="11" t="s">
         <v>7</v>
       </c>
@@ -27540,7 +27534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="11" t="s">
         <v>7</v>
       </c>
@@ -27575,7 +27569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="11" t="s">
         <v>7</v>
       </c>
@@ -27610,7 +27604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A139" s="11" t="s">
         <v>7</v>
       </c>
@@ -27645,7 +27639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A140" s="11" t="s">
         <v>7</v>
       </c>
@@ -27680,7 +27674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="11" t="s">
         <v>7</v>
       </c>
@@ -27715,7 +27709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="11" t="s">
         <v>7</v>
       </c>
@@ -27750,7 +27744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="11" t="s">
         <v>7</v>
       </c>
@@ -27785,7 +27779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="11" t="s">
         <v>7</v>
       </c>
@@ -27820,7 +27814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="11" t="s">
         <v>7</v>
       </c>
@@ -27855,7 +27849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="11" t="s">
         <v>7</v>
       </c>
@@ -27890,7 +27884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="11" t="s">
         <v>7</v>
       </c>
@@ -27925,7 +27919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="11" t="s">
         <v>7</v>
       </c>
@@ -27960,7 +27954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="11" t="s">
         <v>7</v>
       </c>
@@ -27995,7 +27989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="11" t="s">
         <v>7</v>
       </c>
@@ -28030,7 +28024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="11" t="s">
         <v>7</v>
       </c>
@@ -28065,7 +28059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="11" t="s">
         <v>7</v>
       </c>
@@ -28100,7 +28094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="11" t="s">
         <v>7</v>
       </c>
@@ -28135,7 +28129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
         <v>7</v>
       </c>
@@ -28170,7 +28164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="11" t="s">
         <v>7</v>
       </c>
@@ -28205,7 +28199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A156" s="11" t="s">
         <v>7</v>
       </c>
@@ -28240,7 +28234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A157" s="11" t="s">
         <v>7</v>
       </c>
@@ -28275,7 +28269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A158" s="11" t="s">
         <v>7</v>
       </c>
@@ -28310,7 +28304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A159" s="11" t="s">
         <v>7</v>
       </c>
@@ -28345,7 +28339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A160" s="11" t="s">
         <v>7</v>
       </c>
@@ -28380,7 +28374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A161" s="11" t="s">
         <v>7</v>
       </c>
@@ -28415,7 +28409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A162" s="11" t="s">
         <v>7</v>
       </c>
@@ -28450,7 +28444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A163" s="11" t="s">
         <v>7</v>
       </c>
@@ -28485,7 +28479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A164" s="11" t="s">
         <v>7</v>
       </c>
@@ -28520,7 +28514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A165" s="11" t="s">
         <v>7</v>
       </c>
@@ -28555,7 +28549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="11" t="s">
         <v>7</v>
       </c>
@@ -28590,7 +28584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A167" s="11" t="s">
         <v>7</v>
       </c>
@@ -28625,7 +28619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A168" s="11" t="s">
         <v>7</v>
       </c>
@@ -28660,7 +28654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A169" s="11" t="s">
         <v>7</v>
       </c>
@@ -28695,7 +28689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A170" s="11" t="s">
         <v>7</v>
       </c>
@@ -28730,7 +28724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A171" s="11" t="s">
         <v>7</v>
       </c>
@@ -28765,7 +28759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A172" s="11" t="s">
         <v>7</v>
       </c>
@@ -28800,7 +28794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A173" s="11" t="s">
         <v>7</v>
       </c>
@@ -28835,7 +28829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A174" s="11" t="s">
         <v>7</v>
       </c>
@@ -28870,7 +28864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:11" ht="18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A175" s="11" t="s">
         <v>7</v>
       </c>
@@ -28905,7 +28899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A176" s="11" t="s">
         <v>16</v>
       </c>
@@ -28940,7 +28934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A177" s="11" t="s">
         <v>16</v>
       </c>
@@ -28975,7 +28969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="11" t="s">
         <v>16</v>
       </c>
@@ -29010,7 +29004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="11" t="s">
         <v>16</v>
       </c>
@@ -29045,7 +29039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A180" s="11" t="s">
         <v>16</v>
       </c>
@@ -29080,7 +29074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A181" s="11" t="s">
         <v>16</v>
       </c>
@@ -29115,7 +29109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A182" s="11" t="s">
         <v>16</v>
       </c>
@@ -29150,7 +29144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A183" s="11" t="s">
         <v>16</v>
       </c>
@@ -29185,7 +29179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="11" t="s">
         <v>16</v>
       </c>
@@ -29220,7 +29214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="11" t="s">
         <v>41</v>
       </c>
@@ -29255,7 +29249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="11" t="s">
         <v>41</v>
       </c>
@@ -29290,7 +29284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="11" t="s">
         <v>41</v>
       </c>
@@ -29325,7 +29319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="11" t="s">
         <v>41</v>
       </c>
@@ -29360,7 +29354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="11" t="s">
         <v>41</v>
       </c>
@@ -29395,7 +29389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="11" t="s">
         <v>41</v>
       </c>
@@ -29430,7 +29424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="11" t="s">
         <v>41</v>
       </c>
@@ -29465,7 +29459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="11" t="s">
         <v>41</v>
       </c>
@@ -29500,7 +29494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="11" t="s">
         <v>41</v>
       </c>
@@ -29535,7 +29529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="11" t="s">
         <v>41</v>
       </c>
@@ -29570,7 +29564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="11" t="s">
         <v>41</v>
       </c>
@@ -29605,7 +29599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="11" t="s">
         <v>41</v>
       </c>
@@ -29640,7 +29634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="11" t="s">
         <v>41</v>
       </c>
@@ -29675,7 +29669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="11" t="s">
         <v>41</v>
       </c>
@@ -29710,7 +29704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="11" t="s">
         <v>41</v>
       </c>
@@ -29745,7 +29739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="11" t="s">
         <v>41</v>
       </c>
@@ -29780,7 +29774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="11" t="s">
         <v>41</v>
       </c>
@@ -29815,7 +29809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="11" t="s">
         <v>41</v>
       </c>
@@ -29850,7 +29844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="11" t="s">
         <v>41</v>
       </c>
@@ -29885,7 +29879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="11" t="s">
         <v>41</v>
       </c>
@@ -29920,7 +29914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="11" t="s">
         <v>41</v>
       </c>
@@ -29955,7 +29949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:11" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="11" t="s">
         <v>41</v>
       </c>
@@ -29990,7 +29984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="11" t="s">
         <v>41</v>
       </c>
@@ -30025,7 +30019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="11" t="s">
         <v>41</v>
       </c>
@@ -30060,7 +30054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="11" t="s">
         <v>41</v>
       </c>
@@ -30095,7 +30089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="11" t="s">
         <v>41</v>
       </c>
@@ -30130,7 +30124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="11" t="s">
         <v>41</v>
       </c>
@@ -30165,7 +30159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="11" t="s">
         <v>41</v>
       </c>
@@ -30200,7 +30194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="11" t="s">
         <v>41</v>
       </c>
@@ -30235,7 +30229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="11" t="s">
         <v>41</v>
       </c>
@@ -30270,7 +30264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="11" t="s">
         <v>41</v>
       </c>
@@ -30305,7 +30299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="11" t="s">
         <v>41</v>
       </c>
@@ -30340,7 +30334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="11" t="s">
         <v>41</v>
       </c>
@@ -30375,7 +30369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="11" t="s">
         <v>41</v>
       </c>
@@ -30410,7 +30404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="11" t="s">
         <v>41</v>
       </c>
@@ -30445,7 +30439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="11" t="s">
         <v>41</v>
       </c>
@@ -30585,7 +30579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="11" t="s">
         <v>41</v>
       </c>
@@ -30620,7 +30614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="11" t="s">
         <v>41</v>
       </c>
@@ -30655,7 +30649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="11" t="s">
         <v>41</v>
       </c>
@@ -30690,7 +30684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="11" t="s">
         <v>41</v>
       </c>
@@ -30725,7 +30719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="11" t="s">
         <v>41</v>
       </c>
@@ -30760,7 +30754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" s="11" t="s">
         <v>41</v>
       </c>
@@ -30795,7 +30789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="11" t="s">
         <v>41</v>
       </c>
@@ -30830,7 +30824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="11" t="s">
         <v>41</v>
       </c>
@@ -30865,7 +30859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="11" t="s">
         <v>41</v>
       </c>
@@ -30900,7 +30894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="11" t="s">
         <v>41</v>
       </c>
@@ -30935,7 +30929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="11" t="s">
         <v>41</v>
       </c>
@@ -30970,7 +30964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="11" t="s">
         <v>41</v>
       </c>
@@ -31005,7 +30999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="11" t="s">
         <v>41</v>
       </c>
@@ -31040,7 +31034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="11" t="s">
         <v>41</v>
       </c>
@@ -31075,7 +31069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" s="11" t="s">
         <v>41</v>
       </c>
@@ -31110,7 +31104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="11" t="s">
         <v>41</v>
       </c>
@@ -31145,7 +31139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" s="11" t="s">
         <v>41</v>
       </c>
@@ -31180,7 +31174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="11" t="s">
         <v>41</v>
       </c>
@@ -31215,7 +31209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="11" t="s">
         <v>41</v>
       </c>
@@ -31250,7 +31244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="11" t="s">
         <v>41</v>
       </c>
@@ -31285,7 +31279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="11" t="s">
         <v>41</v>
       </c>
@@ -31320,7 +31314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="11" t="s">
         <v>41</v>
       </c>
@@ -31355,7 +31349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="11" t="s">
         <v>41</v>
       </c>
@@ -31390,7 +31384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" s="11" t="s">
         <v>41</v>
       </c>
@@ -31425,7 +31419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="11" t="s">
         <v>41</v>
       </c>
@@ -31460,7 +31454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" s="11" t="s">
         <v>41</v>
       </c>
@@ -31495,7 +31489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" s="11" t="s">
         <v>41</v>
       </c>
@@ -31530,7 +31524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" s="11" t="s">
         <v>41</v>
       </c>
@@ -31565,7 +31559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" s="11" t="s">
         <v>41</v>
       </c>
@@ -31600,7 +31594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" s="11" t="s">
         <v>41</v>
       </c>
@@ -31635,7 +31629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="11" t="s">
         <v>41</v>
       </c>
@@ -31670,7 +31664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" s="11" t="s">
         <v>41</v>
       </c>
@@ -31705,7 +31699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" s="11" t="s">
         <v>41</v>
       </c>
@@ -31740,7 +31734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257" s="11" t="s">
         <v>41</v>
       </c>
@@ -31775,7 +31769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" s="11" t="s">
         <v>46</v>
       </c>
@@ -31810,7 +31804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259" s="11" t="s">
         <v>46</v>
       </c>
@@ -31845,7 +31839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" s="11" t="s">
         <v>46</v>
       </c>
@@ -31880,7 +31874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A261" s="11" t="s">
         <v>46</v>
       </c>
@@ -31915,7 +31909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" s="11" t="s">
         <v>46</v>
       </c>
@@ -31950,7 +31944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" s="11" t="s">
         <v>46</v>
       </c>
@@ -31985,7 +31979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" s="11" t="s">
         <v>46</v>
       </c>
@@ -32020,7 +32014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265" s="11" t="s">
         <v>46</v>
       </c>
@@ -32055,7 +32049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" s="11" t="s">
         <v>46</v>
       </c>
@@ -32090,7 +32084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267" s="11" t="s">
         <v>46</v>
       </c>
@@ -32125,7 +32119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268" s="11" t="s">
         <v>46</v>
       </c>
@@ -32160,7 +32154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" s="11" t="s">
         <v>46</v>
       </c>
@@ -32195,7 +32189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" s="11" t="s">
         <v>46</v>
       </c>
@@ -32230,7 +32224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271" s="11" t="s">
         <v>46</v>
       </c>
@@ -32265,7 +32259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" s="11" t="s">
         <v>46</v>
       </c>
@@ -32300,7 +32294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273" s="11" t="s">
         <v>46</v>
       </c>
@@ -32335,7 +32329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" s="11" t="s">
         <v>46</v>
       </c>
@@ -32370,7 +32364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275" s="11" t="s">
         <v>46</v>
       </c>
@@ -32405,7 +32399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" s="11" t="s">
         <v>46</v>
       </c>
@@ -32440,7 +32434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" s="11" t="s">
         <v>46</v>
       </c>
@@ -32475,7 +32469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" s="11" t="s">
         <v>46</v>
       </c>
@@ -32510,7 +32504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" s="11" t="s">
         <v>46</v>
       </c>
@@ -32545,7 +32539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" s="11" t="s">
         <v>46</v>
       </c>
@@ -32580,7 +32574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" s="11" t="s">
         <v>46</v>
       </c>
@@ -32615,7 +32609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" s="11" t="s">
         <v>46</v>
       </c>
@@ -32650,7 +32644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" s="11" t="s">
         <v>46</v>
       </c>
@@ -32685,7 +32679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" s="11" t="s">
         <v>46</v>
       </c>
@@ -32720,7 +32714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" s="11" t="s">
         <v>46</v>
       </c>
@@ -32755,7 +32749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286" s="11" t="s">
         <v>46</v>
       </c>
@@ -32790,7 +32784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287" s="11" t="s">
         <v>46</v>
       </c>
@@ -32825,7 +32819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" s="11" t="s">
         <v>46</v>
       </c>
@@ -32860,7 +32854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289" s="11" t="s">
         <v>46</v>
       </c>
@@ -32895,7 +32889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" s="11" t="s">
         <v>46</v>
       </c>
@@ -32930,7 +32924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A291" s="11" t="s">
         <v>46</v>
       </c>
@@ -32965,7 +32959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A292" s="11" t="s">
         <v>46</v>
       </c>
@@ -33000,7 +32994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A293" s="11" t="s">
         <v>46</v>
       </c>
@@ -33035,7 +33029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A294" s="11" t="s">
         <v>46</v>
       </c>
@@ -33070,7 +33064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A295" s="11" t="s">
         <v>46</v>
       </c>
@@ -33105,7 +33099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A296" s="11" t="s">
         <v>46</v>
       </c>
@@ -33140,7 +33134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A297" s="11" t="s">
         <v>46</v>
       </c>
@@ -33175,7 +33169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A298" s="11" t="s">
         <v>46</v>
       </c>
@@ -33210,7 +33204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A299" s="11" t="s">
         <v>46</v>
       </c>
@@ -33245,7 +33239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A300" s="11" t="s">
         <v>46</v>
       </c>
@@ -33280,7 +33274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A301" s="11" t="s">
         <v>46</v>
       </c>
@@ -33315,7 +33309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A302" s="11" t="s">
         <v>46</v>
       </c>
@@ -33350,7 +33344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A303" s="11" t="s">
         <v>46</v>
       </c>
@@ -33385,7 +33379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304" s="11" t="s">
         <v>46</v>
       </c>
@@ -33420,7 +33414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A305" s="11" t="s">
         <v>46</v>
       </c>
@@ -33455,7 +33449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306" s="11" t="s">
         <v>46</v>
       </c>
@@ -33490,7 +33484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A307" s="11" t="s">
         <v>46</v>
       </c>
@@ -33525,7 +33519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" s="11" t="s">
         <v>46</v>
       </c>
@@ -33560,7 +33554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A309" s="11" t="s">
         <v>46</v>
       </c>
@@ -33595,7 +33589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A310" s="11" t="s">
         <v>46</v>
       </c>
@@ -33630,7 +33624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A311" s="11" t="s">
         <v>46</v>
       </c>
@@ -33665,7 +33659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A312" s="11" t="s">
         <v>46</v>
       </c>
@@ -33700,7 +33694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A313" s="11" t="s">
         <v>46</v>
       </c>
@@ -33735,7 +33729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A314" s="11" t="s">
         <v>46</v>
       </c>
@@ -33770,7 +33764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A315" s="11" t="s">
         <v>46</v>
       </c>
@@ -33805,7 +33799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316" s="11" t="s">
         <v>46</v>
       </c>
@@ -33840,7 +33834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317" s="11" t="s">
         <v>46</v>
       </c>
@@ -33875,7 +33869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" s="11" t="s">
         <v>46</v>
       </c>
@@ -33910,7 +33904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A319" s="11" t="s">
         <v>46</v>
       </c>
@@ -33946,16 +33940,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:K319" xr:uid="{2460B869-2CC9-4C96-B69B-2FCDE5601999}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Object-Oriented Changes"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A8:K319">
-      <sortCondition ref="A7"/>
-    </sortState>
-  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:E4"/>
@@ -33967,11 +33951,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA45B255-BEC9-4DE2-B957-9F984FFC1ACD}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="9" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -34036,7 +34019,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
@@ -34065,7 +34048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
@@ -34094,7 +34077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
@@ -34123,7 +34106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>6</v>
       </c>
@@ -34152,7 +34135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
@@ -34181,7 +34164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>6</v>
       </c>
@@ -34210,7 +34193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>6</v>
       </c>
@@ -34239,7 +34222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>6</v>
       </c>
@@ -34268,7 +34251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>6</v>
       </c>
@@ -34297,7 +34280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>6</v>
       </c>
@@ -34326,7 +34309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>6</v>
       </c>
@@ -34355,7 +34338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>6</v>
       </c>
@@ -34384,7 +34367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>6</v>
       </c>
@@ -34413,7 +34396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>6</v>
       </c>
@@ -34442,7 +34425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>6</v>
       </c>
@@ -34471,7 +34454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>6</v>
       </c>
@@ -34500,7 +34483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>6</v>
       </c>
@@ -34529,7 +34512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>6</v>
       </c>
@@ -34558,7 +34541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>279</v>
       </c>
@@ -34587,7 +34570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>279</v>
       </c>
@@ -34616,7 +34599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>279</v>
       </c>
@@ -34645,7 +34628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>279</v>
       </c>
@@ -34674,7 +34657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>279</v>
       </c>
@@ -34703,7 +34686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>279</v>
       </c>
@@ -34732,7 +34715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>279</v>
       </c>
@@ -34761,7 +34744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>279</v>
       </c>
@@ -34790,7 +34773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>279</v>
       </c>
@@ -34819,7 +34802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>279</v>
       </c>
@@ -34848,7 +34831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>7</v>
       </c>
@@ -34877,7 +34860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>7</v>
       </c>
@@ -34906,7 +34889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>7</v>
       </c>
@@ -34935,7 +34918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>7</v>
       </c>
@@ -34964,7 +34947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>7</v>
       </c>
@@ -34993,7 +34976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>7</v>
       </c>
@@ -35022,7 +35005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>7</v>
       </c>
@@ -35051,7 +35034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>7</v>
       </c>
@@ -35080,7 +35063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="14" customFormat="1" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="14" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>7</v>
       </c>
@@ -35109,7 +35092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="14" customFormat="1" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="14" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>7</v>
       </c>
@@ -35138,7 +35121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>7</v>
       </c>
@@ -35167,7 +35150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>7</v>
       </c>
@@ -35196,7 +35179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>7</v>
       </c>
@@ -35225,7 +35208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="27" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>7</v>
       </c>
@@ -35254,7 +35237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>7</v>
       </c>
@@ -35283,7 +35266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>7</v>
       </c>
@@ -35312,7 +35295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>7</v>
       </c>
@@ -35341,7 +35324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>7</v>
       </c>
@@ -35370,7 +35353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>7</v>
       </c>
@@ -35399,7 +35382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>7</v>
       </c>
@@ -35428,7 +35411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>7</v>
       </c>
@@ -35457,7 +35440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>7</v>
       </c>
@@ -35486,7 +35469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="27" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>16</v>
       </c>
@@ -35515,7 +35498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="27" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>16</v>
       </c>
@@ -35544,7 +35527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>16</v>
       </c>
@@ -35573,7 +35556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="27" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
         <v>16</v>
       </c>
@@ -35602,7 +35585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
         <v>16</v>
       </c>
@@ -35631,7 +35614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>41</v>
       </c>
@@ -35660,7 +35643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>41</v>
       </c>
@@ -35689,7 +35672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>41</v>
       </c>
@@ -35718,7 +35701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>41</v>
       </c>
@@ -35747,7 +35730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>41</v>
       </c>
@@ -35776,7 +35759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>41</v>
       </c>
@@ -35805,7 +35788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>41</v>
       </c>
@@ -35834,7 +35817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>41</v>
       </c>
@@ -35863,7 +35846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>41</v>
       </c>
@@ -35892,7 +35875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>41</v>
       </c>
@@ -35921,7 +35904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>41</v>
       </c>
@@ -35950,7 +35933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>41</v>
       </c>
@@ -35979,7 +35962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>41</v>
       </c>
@@ -36008,7 +35991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>41</v>
       </c>
@@ -36037,7 +36020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>41</v>
       </c>
@@ -36066,7 +36049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>41</v>
       </c>
@@ -36095,7 +36078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>41</v>
       </c>
@@ -36124,7 +36107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
         <v>41</v>
       </c>
@@ -36211,7 +36194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>41</v>
       </c>
@@ -36240,7 +36223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
         <v>41</v>
       </c>
@@ -36269,7 +36252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
         <v>41</v>
       </c>
@@ -36298,7 +36281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>41</v>
       </c>
@@ -36327,7 +36310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>41</v>
       </c>
@@ -36356,7 +36339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
         <v>41</v>
       </c>
@@ -36385,7 +36368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
         <v>41</v>
       </c>
@@ -36414,7 +36397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
         <v>41</v>
       </c>
@@ -36443,7 +36426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
         <v>41</v>
       </c>
@@ -36472,7 +36455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
         <v>41</v>
       </c>
@@ -36501,7 +36484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
         <v>41</v>
       </c>
@@ -36530,7 +36513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
         <v>41</v>
       </c>
@@ -36559,7 +36542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
         <v>41</v>
       </c>
@@ -36588,7 +36571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
         <v>41</v>
       </c>
@@ -36617,7 +36600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
         <v>41</v>
       </c>
@@ -36646,7 +36629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
         <v>41</v>
       </c>
@@ -36675,7 +36658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
         <v>46</v>
       </c>
@@ -36704,7 +36687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
         <v>46</v>
       </c>
@@ -36733,7 +36716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
         <v>46</v>
       </c>
@@ -36762,7 +36745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
         <v>46</v>
       </c>
@@ -36791,7 +36774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
         <v>46</v>
       </c>
@@ -36820,7 +36803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
         <v>46</v>
       </c>
@@ -36849,7 +36832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
         <v>46</v>
       </c>
@@ -36878,7 +36861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
         <v>46</v>
       </c>
@@ -36907,7 +36890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
         <v>46</v>
       </c>
@@ -36936,7 +36919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
         <v>46</v>
       </c>
@@ -36965,7 +36948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
         <v>46</v>
       </c>
@@ -36994,7 +36977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
         <v>46</v>
       </c>
@@ -37023,7 +37006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
         <v>46</v>
       </c>
@@ -37053,16 +37036,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:I111" xr:uid="{C7CC5BDA-2564-4B44-92E8-06046A786115}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Object-Oriented Changes"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A8:I111">
-      <sortCondition ref="A7"/>
-    </sortState>
-  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:E4"/>
@@ -37079,8 +37052,8 @@
   </sheetPr>
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="9" outlineLevelRow="2" x14ac:dyDescent="0.25"/>

</xml_diff>